<commit_message>
MAJ DOCS, Livert Non Clos
</commit_message>
<xml_diff>
--- a/LstDocuments.xlsx
+++ b/LstDocuments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\2pConsultants\EHESP\APP\gestVAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04B6711-7819-4BDA-9936-60FFA63B8060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEA0205-5299-45CB-982F-AEF5A4CC59D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10785" xr2:uid="{2FEE0C03-3F36-4513-B9E0-E713BA8A6B24}"/>
   </bookViews>
@@ -195,8 +195,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -212,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -220,12 +228,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,417 +569,444 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89636BC-C404-4244-8597-D65BDA84A16E}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="D34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>